<commit_message>
AKA changes to sdCard to be saved while merged with Johns
</commit_message>
<xml_diff>
--- a/Documentation/AQ32Plus Timing.xlsx
+++ b/Documentation/AQ32Plus Timing.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4507"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="120" yWindow="45" windowWidth="18195" windowHeight="7230"/>
@@ -11,12 +11,12 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Hz</t>
   </si>
@@ -35,12 +35,18 @@
   <si>
     <t>AQ32 + MTK Binary</t>
   </si>
+  <si>
+    <t>AQ32 + LA Timing</t>
+  </si>
+  <si>
+    <t>199 when doing CLI output</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -98,6 +104,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -193,7 +202,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -228,7 +236,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -404,31 +411,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="L15" sqref="L15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="C1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="6"/>
+      <c r="D1" s="7"/>
       <c r="E1" s="1"/>
       <c r="H1" s="5" t="s">
         <v>0</v>
@@ -436,13 +443,13 @@
       <c r="I1" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="K1" s="6"/>
+      <c r="K1" s="7"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12">
       <c r="A2">
         <v>1000</v>
       </c>
@@ -480,7 +487,7 @@
         <v>0.28955599999999998</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12">
       <c r="A3">
         <v>500</v>
       </c>
@@ -510,7 +517,7 @@
         <v>5.8000000000000003E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12">
       <c r="A4">
         <v>100</v>
       </c>
@@ -540,7 +547,7 @@
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12">
       <c r="A5">
         <v>50</v>
       </c>
@@ -570,7 +577,7 @@
         <v>2.0000000000000001E-4</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12">
       <c r="A6">
         <v>10</v>
       </c>
@@ -600,7 +607,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12">
       <c r="A7">
         <v>5</v>
       </c>
@@ -630,7 +637,7 @@
         <v>5.0000000000000004E-6</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12">
       <c r="A8">
         <v>1</v>
       </c>
@@ -660,25 +667,31 @@
         <v>9.9999999999999995E-7</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12">
       <c r="A10" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B10" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D10" s="6"/>
+      <c r="D10" s="7"/>
       <c r="E10" s="5"/>
-      <c r="H10" s="5"/>
-      <c r="I10" s="5"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="6"/>
-      <c r="L10" s="5"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H10" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="I10" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="K10" s="7"/>
+      <c r="L10" s="6"/>
+    </row>
+    <row r="11" spans="1:12">
       <c r="A11">
         <v>1000</v>
       </c>
@@ -697,10 +710,23 @@
         <f>SUM(D11:D17)</f>
         <v>0.29466000000000003</v>
       </c>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <v>1000</v>
+      </c>
+      <c r="I11">
+        <f>1/H11*1000000</f>
+        <v>1000</v>
+      </c>
+      <c r="K11" s="3">
+        <f>J11/I11</f>
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <f>SUM(K11:K17)</f>
+        <v>3.5192500000000008E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12">
       <c r="A12">
         <v>500</v>
       </c>
@@ -715,9 +741,22 @@
         <f t="shared" ref="D12:D17" si="5">C12/B12</f>
         <v>5.3499999999999999E-2</v>
       </c>
-      <c r="K12" s="3"/>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <v>500</v>
+      </c>
+      <c r="I12">
+        <f t="shared" ref="I12:I17" si="6">1/H12*1000000</f>
+        <v>2000</v>
+      </c>
+      <c r="J12">
+        <v>66</v>
+      </c>
+      <c r="K12" s="3">
+        <f t="shared" ref="K12:K17" si="7">J12/I12</f>
+        <v>3.3000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12">
       <c r="A13">
         <v>100</v>
       </c>
@@ -732,9 +771,22 @@
         <f t="shared" si="5"/>
         <v>1.4E-3</v>
       </c>
-      <c r="K13" s="3"/>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <v>100</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="6"/>
+        <v>10000</v>
+      </c>
+      <c r="J13">
+        <v>13</v>
+      </c>
+      <c r="K13" s="3">
+        <f t="shared" si="7"/>
+        <v>1.2999999999999999E-3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12">
       <c r="A14">
         <v>50</v>
       </c>
@@ -749,9 +801,22 @@
         <f t="shared" si="5"/>
         <v>8.0499999999999999E-3</v>
       </c>
-      <c r="K14" s="3"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H14">
+        <v>50</v>
+      </c>
+      <c r="I14">
+        <f t="shared" si="6"/>
+        <v>20000</v>
+      </c>
+      <c r="J14">
+        <v>4.5</v>
+      </c>
+      <c r="K14" s="3">
+        <f t="shared" si="7"/>
+        <v>2.2499999999999999E-4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12">
       <c r="A15">
         <v>10</v>
       </c>
@@ -766,9 +831,25 @@
         <f t="shared" si="5"/>
         <v>7.1000000000000002E-4</v>
       </c>
-      <c r="K15" s="3"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H15">
+        <v>10</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="6"/>
+        <v>100000</v>
+      </c>
+      <c r="J15">
+        <v>66</v>
+      </c>
+      <c r="K15" s="3">
+        <f t="shared" si="7"/>
+        <v>6.6E-4</v>
+      </c>
+      <c r="L15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12">
       <c r="A16">
         <v>5</v>
       </c>
@@ -783,9 +864,22 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K16" s="3"/>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H16">
+        <v>5</v>
+      </c>
+      <c r="I16">
+        <f t="shared" si="6"/>
+        <v>200000</v>
+      </c>
+      <c r="J16">
+        <v>1.5</v>
+      </c>
+      <c r="K16" s="3">
+        <f t="shared" si="7"/>
+        <v>7.5000000000000002E-6</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12">
       <c r="A17">
         <v>1</v>
       </c>
@@ -800,27 +894,37 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="K17" s="3"/>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H17">
+        <v>1</v>
+      </c>
+      <c r="I17">
+        <f t="shared" si="6"/>
+        <v>1000000</v>
+      </c>
+      <c r="K17" s="3">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12">
       <c r="A19" s="5" t="s">
         <v>0</v>
       </c>
       <c r="B19" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="D19" s="6"/>
+      <c r="D19" s="7"/>
       <c r="E19" s="5"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
-      <c r="J19" s="6"/>
-      <c r="K19" s="6"/>
+      <c r="J19" s="7"/>
+      <c r="K19" s="7"/>
       <c r="L19" s="5"/>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12">
       <c r="A20">
         <v>1000</v>
       </c>
@@ -842,113 +946,113 @@
       <c r="K20" s="3"/>
       <c r="L20" s="3"/>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12">
       <c r="A21">
         <v>500</v>
       </c>
       <c r="B21">
-        <f t="shared" ref="B21:B26" si="6">1/A21*1000000</f>
+        <f t="shared" ref="B21:B26" si="8">1/A21*1000000</f>
         <v>2000</v>
       </c>
       <c r="C21">
         <v>116</v>
       </c>
       <c r="D21" s="3">
-        <f t="shared" ref="D21:D26" si="7">C21/B21</f>
+        <f t="shared" ref="D21:D26" si="9">C21/B21</f>
         <v>5.8000000000000003E-2</v>
       </c>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12">
       <c r="A22">
         <v>100</v>
       </c>
       <c r="B22">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>10000</v>
       </c>
       <c r="C22">
         <v>3</v>
       </c>
       <c r="D22" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.9999999999999997E-4</v>
       </c>
       <c r="K22" s="3"/>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12">
       <c r="A23">
         <v>50</v>
       </c>
       <c r="B23">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20000</v>
       </c>
       <c r="C23">
         <v>4</v>
       </c>
       <c r="D23" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>2.0000000000000001E-4</v>
       </c>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12">
       <c r="A24">
         <v>10</v>
       </c>
       <c r="B24">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>100000</v>
       </c>
       <c r="C24">
         <v>5</v>
       </c>
       <c r="D24" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="K24" s="3"/>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12">
       <c r="A25">
         <v>5</v>
       </c>
       <c r="B25">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>200000</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>5.0000000000000004E-6</v>
       </c>
       <c r="K25" s="3"/>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12">
       <c r="A26">
         <v>1</v>
       </c>
       <c r="B26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>1000000</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" s="3">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>9.9999999999999995E-7</v>
       </c>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12">
       <c r="C27" s="4"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12">
       <c r="C28" s="4"/>
     </row>
   </sheetData>
@@ -966,24 +1070,24 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added _DTIMING debug defines in the 1000hz interrupt, updated the time stamp in the logoutput to include 5 digits after the decimal point
</commit_message>
<xml_diff>
--- a/Documentation/AQ32Plus Timing.xlsx
+++ b/Documentation/AQ32Plus Timing.xlsx
@@ -415,7 +415,7 @@
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -717,13 +717,16 @@
         <f>1/H11*1000000</f>
         <v>1000</v>
       </c>
+      <c r="J11">
+        <v>233</v>
+      </c>
       <c r="K11" s="3">
         <f>J11/I11</f>
-        <v>0</v>
+        <v>0.23300000000000001</v>
       </c>
       <c r="L11" s="3">
         <f>SUM(K11:K17)</f>
-        <v>3.5192500000000008E-2</v>
+        <v>0.26971349999999999</v>
       </c>
     </row>
     <row r="12" spans="1:12">
@@ -749,11 +752,11 @@
         <v>2000</v>
       </c>
       <c r="J12">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="K12" s="3">
         <f t="shared" ref="K12:K17" si="7">J12/I12</f>
-        <v>3.3000000000000002E-2</v>
+        <v>3.4500000000000003E-2</v>
       </c>
     </row>
     <row r="13" spans="1:12">
@@ -809,11 +812,11 @@
         <v>20000</v>
       </c>
       <c r="J14">
-        <v>4.5</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="K14" s="3">
         <f t="shared" si="7"/>
-        <v>2.2499999999999999E-4</v>
+        <v>2.4499999999999999E-4</v>
       </c>
     </row>
     <row r="15" spans="1:12">
@@ -901,9 +904,12 @@
         <f t="shared" si="6"/>
         <v>1000000</v>
       </c>
+      <c r="J17">
+        <v>1</v>
+      </c>
       <c r="K17" s="3">
         <f t="shared" si="7"/>
-        <v>0</v>
+        <v>9.9999999999999995E-7</v>
       </c>
     </row>
     <row r="19" spans="1:12">

</xml_diff>